<commit_message>
Copy Files From Source Repo (2024-07-19 18:35)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -52,56 +52,61 @@
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>차이 티 총 판매량(개)</t>
+      <t>총 Chai 판매(개수)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>수제 차이 티 판매량(개)</t>
+      <t>Artisanal Chai 판매(단위)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>즉석 음용 차이 티 판매량(개)</t>
+      <t>미리 만든 Chai 판매(단위)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>소셜 미디어 참여율(조회수)</t>
+      <t>소셜 미디어 참여도(보기)</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>온라인 차이 티 검색 수</t>
+      <t>Chai에 대한 온라인 검색</t>
     </r>
   </si>
   <si>
@@ -123,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +152,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -434,11 +433,11 @@
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="날짜" dataDxfId="0"/>
-    <tableColumn id="2" name="차이 티 총 판매량(개)"/>
-    <tableColumn id="3" name="수제 차이 티 판매량(개)"/>
-    <tableColumn id="4" name="즉석 음용 차이 티 판매량(개)"/>
-    <tableColumn id="5" name="소셜 미디어 참여율(조회수)"/>
-    <tableColumn id="6" name="온라인 차이 티 검색 수"/>
+    <tableColumn id="2" name="총 Chai 판매(개수)"/>
+    <tableColumn id="3" name="Artisanal Chai 판매(단위)"/>
+    <tableColumn id="4" name="미리 만든 Chai 판매(단위)"/>
+    <tableColumn id="5" name="소셜 미디어 참여도(보기)"/>
+    <tableColumn id="6" name="Chai에 대한 온라인 검색"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>

<commit_message>
Copy Files From Source Repo (2025-02-12 19:15)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <r>
       <rPr>
@@ -58,7 +58,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>총 Chai 판매(개수)</t>
+      <t>총 차이 판매액(단위)</t>
     </r>
   </si>
   <si>
@@ -118,6 +118,17 @@
         <family val="2"/>
       </rPr>
       <t>46-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>5:48</t>
     </r>
   </si>
 </sst>
@@ -433,7 +444,7 @@
   <autoFilter ref="A1:F14"/>
   <tableColumns count="6">
     <tableColumn id="1" name="날짜" dataDxfId="0"/>
-    <tableColumn id="2" name="총 Chai 판매(개수)"/>
+    <tableColumn id="2" name="총 차이 판매액(단위)"/>
     <tableColumn id="3" name="Artisanal Chai 판매(단위)"/>
     <tableColumn id="4" name="미리 만든 Chai 판매(단위)"/>
     <tableColumn id="5" name="소셜 미디어 참여도(보기)"/>
@@ -882,8 +893,8 @@
       <c r="C7">
         <v>315</v>
       </c>
-      <c r="D7">
-        <v>548</v>
+      <c r="D7" t="s">
+        <v>7</v>
       </c>
       <c r="E7">
         <v>3599</v>

</xml_diff>